<commit_message>
Clean up a bit Huawei algorithm.
</commit_message>
<xml_diff>
--- a/Supported networks.xlsx
+++ b/Supported networks.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="25520" yWindow="-1600" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Hoja1!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="83">
   <si>
     <t>ESSID</t>
   </si>
@@ -127,13 +130,154 @@
   </si>
   <si>
     <t>Tecom</t>
+  </si>
+  <si>
+    <t>Encryption</t>
+  </si>
+  <si>
+    <t>WPA</t>
+  </si>
+  <si>
+    <t>Any?</t>
+  </si>
+  <si>
+    <t>Search encryption…</t>
+  </si>
+  <si>
+    <t>00:25:68:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>Visto en HG520 español</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>Visto en routerkeygen</t>
+  </si>
+  <si>
+    <t>Yes?</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>HG265</t>
+  </si>
+  <si>
+    <t>Visto en Telmex, HG530 (pero en vodafone no funciona!!!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Visto a varias VodafoneXXXX</t>
+  </si>
+  <si>
+    <t>Huawei wa1003A</t>
+  </si>
+  <si>
+    <t>Por lo visto es el que tiene el Huawei U8100/8150, y otros routers</t>
+  </si>
+  <si>
+    <t>Visto en algunas Vodafone, pero tb en Orange</t>
+  </si>
+  <si>
+    <t>Es de Orange, no comercializa ese router</t>
+  </si>
+  <si>
+    <t>VodafoneInternetMovil</t>
+  </si>
+  <si>
+    <t>00:25:9E:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>04:C0:6F:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>08:19:A6:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>0C:37:DC:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>10:C6:1F:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>1C:1D:67:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>20:2B:C1:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>20:F3:A3:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>24:DB:AC:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>28:5F:DB:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>28:6E:D4:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>30:87:30:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>40:4D:8E:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>4C:54:99:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>4C:1F:CC:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>54:A5:1B:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>54:89:98:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>64:16:F0:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>00:E0:FC:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>00:18:82:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>00:0F:E2:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>00:11:F5:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>F4:C7:14:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>78:1D:BA:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>5C:4C:A9:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>00:1E:10:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>00:22:A1:XX:XX:XX</t>
+  </si>
+  <si>
+    <t>Huawei HG520c</t>
+  </si>
+  <si>
+    <t>Viewed in routerkeygen...</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,13 +301,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -175,17 +350,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -515,85 +721,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:E21"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="52.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>20</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -601,229 +825,743 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1">
+      <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1">
+      <c r="A21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="3" customFormat="1">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="3" customFormat="1">
+      <c r="A24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1">
+      <c r="A25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1">
+      <c r="A26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1">
+      <c r="A27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1">
+      <c r="A28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1">
+      <c r="A29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1">
+      <c r="A30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1">
+      <c r="A31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1">
+      <c r="A32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1">
+      <c r="A33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="3" customFormat="1">
+      <c r="A34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1">
+      <c r="A35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1">
+      <c r="A36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1">
+      <c r="A37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="3" customFormat="1">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1">
+      <c r="A39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="3" customFormat="1">
+      <c r="A40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1">
+      <c r="A41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1">
+      <c r="A42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1">
+      <c r="A43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="3" customFormat="1">
+      <c r="A44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1">
+      <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="3" customFormat="1">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1">
+      <c r="A47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="3" customFormat="1">
+      <c r="A48" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="2" customFormat="1">
+      <c r="A49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="3" customFormat="1">
+      <c r="A50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="2" customFormat="1">
+      <c r="A51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <sortState ref="A2:F20">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="6" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
I think Dlink, Andared and Discuss algorithms are done.
</commit_message>
<xml_diff>
--- a/Supported networks.xlsx
+++ b/Supported networks.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="83">
   <si>
     <t>ESSID</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>WEP/WPA</t>
+  </si>
+  <si>
+    <t>http://pastebin.com/gVkPM1v0, Search more...</t>
   </si>
 </sst>
 </file>
@@ -800,6 +803,9 @@
       <c r="E4" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Fix one error in Comtrend algorithm.
</commit_message>
<xml_diff>
--- a/Supported networks.xlsx
+++ b/Supported networks.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="85">
   <si>
     <t>ESSID</t>
   </si>
@@ -270,7 +270,13 @@
     <t>WEP/WPA</t>
   </si>
   <si>
-    <t>http://pastebin.com/gVkPM1v0, Search more...</t>
+    <t>Es de Orange, no comercializa ese router… mac2wepkey http://pastebin.com/CgqMdXgC</t>
+  </si>
+  <si>
+    <t>WPA magic key</t>
+  </si>
+  <si>
+    <t>Comtrend?/Zyxel?</t>
   </si>
 </sst>
 </file>
@@ -344,8 +350,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -368,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="29">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -377,6 +395,12 @@
     <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -385,6 +409,12 @@
     <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -714,11 +744,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -728,7 +758,7 @@
     <col min="3" max="3" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="54.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -803,9 +833,6 @@
       <c r="E4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
@@ -821,7 +848,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -832,10 +859,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -843,7 +873,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>32</v>
@@ -854,50 +884,53 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -905,16 +938,16 @@
         <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -922,16 +955,13 @@
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -939,7 +969,7 @@
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>
@@ -953,13 +983,16 @@
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -967,16 +1000,13 @@
         <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -984,7 +1014,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
@@ -995,27 +1025,27 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>20</v>
@@ -1023,16 +1053,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1046,41 +1079,38 @@
         <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1094,7 +1124,7 @@
         <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1102,13 +1132,13 @@
         <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1116,7 +1146,7 @@
         <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>40</v>
@@ -1136,7 +1166,7 @@
         <v>40</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1144,13 +1174,13 @@
         <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1158,13 +1188,16 @@
         <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1172,16 +1205,13 @@
         <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1189,7 +1219,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>40</v>
@@ -1203,7 +1233,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>40</v>
@@ -1217,7 +1247,7 @@
         <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>40</v>
@@ -1231,7 +1261,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>40</v>
@@ -1245,13 +1275,16 @@
         <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1259,16 +1292,16 @@
         <v>43</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1276,7 +1309,7 @@
         <v>43</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>40</v>
@@ -1285,24 +1318,24 @@
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1313,61 +1346,61 @@
         <v>9</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>80</v>
+        <v>11</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1375,10 +1408,10 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>11</v>
@@ -1389,87 +1422,84 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>79</v>
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1477,60 +1507,29 @@
         <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update list of wireless networks.
</commit_message>
<xml_diff>
--- a/Supported networks.xlsx
+++ b/Supported networks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25520" yWindow="-1600" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="1380" windowWidth="24920" windowHeight="12980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="89">
   <si>
     <t>ESSID</t>
   </si>
@@ -283,13 +283,19 @@
   </si>
   <si>
     <t>Reports</t>
+  </si>
+  <si>
+    <t>WLAN_XX</t>
+  </si>
+  <si>
+    <t>More than 1 password…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,8 +332,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,6 +359,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -356,7 +375,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -386,13 +405,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="61">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -407,6 +459,22 @@
     <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -421,6 +489,22 @@
     <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -750,11 +834,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9:G49"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1562,99 +1646,105 @@
         <v>37</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1662,7 +1752,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>12</v>
@@ -1674,7 +1764,7 @@
         <v>37</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
@@ -1682,25 +1772,25 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1708,10 +1798,10 @@
         <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>20</v>
@@ -1723,18 +1813,18 @@
         <v>0</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>20</v>
@@ -1746,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1754,7 +1844,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>40</v>
@@ -1767,9 +1857,6 @@
       </c>
       <c r="G46" s="1">
         <v>0</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1777,7 +1864,7 @@
         <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>40</v>
@@ -1794,13 +1881,13 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>20</v>
@@ -1811,28 +1898,8 @@
       <c r="G48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="1">
-        <v>0</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>29</v>
+      <c r="H48" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change pattern style and update supported networks database.
</commit_message>
<xml_diff>
--- a/Supported networks.xlsx
+++ b/Supported networks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="1380" windowWidth="24920" windowHeight="12980" tabRatio="500"/>
+    <workbookView xWindow="27680" yWindow="-840" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="94">
   <si>
     <t>ESSID</t>
   </si>
@@ -289,6 +289,21 @@
   </si>
   <si>
     <t>More than 1 password…</t>
+  </si>
+  <si>
+    <t>WLANXXXXXX</t>
+  </si>
+  <si>
+    <t>WIFIXXXXXX</t>
+  </si>
+  <si>
+    <t>YACOMXXXXXX</t>
+  </si>
+  <si>
+    <t>WLan6X</t>
+  </si>
+  <si>
+    <t>Search encryption…</t>
   </si>
 </sst>
 </file>
@@ -375,8 +390,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,7 +467,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="69">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -475,6 +498,10 @@
     <cellStyle name="Hipervínculo" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -505,6 +532,10 @@
     <cellStyle name="Hipervínculo visitado" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -834,11 +865,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -952,68 +983,71 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1021,7 +1055,7 @@
         <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>40</v>
@@ -1036,53 +1070,50 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1090,7 +1121,7 @@
         <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>40</v>
@@ -1105,24 +1136,27 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -1133,7 +1167,7 @@
         <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>40</v>
@@ -1147,19 +1181,22 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>20</v>
@@ -1168,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1176,7 +1213,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>40</v>
@@ -1196,7 +1233,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
@@ -1213,36 +1250,39 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>20</v>
@@ -1256,7 +1296,7 @@
         <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>40</v>
@@ -1270,19 +1310,16 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>20</v>
@@ -1292,9 +1329,6 @@
       </c>
       <c r="G20" s="1">
         <v>0</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1302,7 +1336,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
@@ -1322,7 +1356,7 @@
         <v>43</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>40</v>
@@ -1336,13 +1370,16 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
+      <c r="H22" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>40</v>
@@ -1355,20 +1392,23 @@
       </c>
       <c r="G23" s="1">
         <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>20</v>
@@ -1382,7 +1422,7 @@
         <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>40</v>
@@ -1402,7 +1442,7 @@
         <v>43</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>40</v>
@@ -1422,7 +1462,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>40</v>
@@ -1442,7 +1482,7 @@
         <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>40</v>
@@ -1456,22 +1496,19 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>20</v>
@@ -1485,7 +1522,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>40</v>
@@ -1505,7 +1542,7 @@
         <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>40</v>
@@ -1519,13 +1556,16 @@
       <c r="G31" s="1">
         <v>0</v>
       </c>
+      <c r="H31" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>40</v>
@@ -1545,7 +1585,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>40</v>
@@ -1565,22 +1605,19 @@
         <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1588,7 +1625,7 @@
         <v>43</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>40</v>
@@ -1602,16 +1639,13 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>40</v>
@@ -1625,34 +1659,28 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1660,7 +1688,7 @@
         <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>40</v>
@@ -1675,136 +1703,139 @@
         <v>0</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>7</v>
+        <v>87</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>20</v>
@@ -1813,47 +1844,50 @@
         <v>0</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G46" s="1">
         <v>0</v>
@@ -1861,13 +1895,13 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>20</v>
@@ -1877,17 +1911,20 @@
       </c>
       <c r="G47" s="1">
         <v>0</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>20</v>
@@ -1899,11 +1936,74 @@
         <v>0</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>88</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F51">
+  <sortState ref="A2:H51">
     <sortCondition descending="1" ref="B1"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Keep insisting in algorithms.
</commit_message>
<xml_diff>
--- a/Supported networks.xlsx
+++ b/Supported networks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27680" yWindow="-840" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="26800" yWindow="-440" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>Discus</t>
   </si>
   <si>
-    <t>Dlink-XXXXXX</t>
-  </si>
-  <si>
     <t>Dlink</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>Search encryption…</t>
+  </si>
+  <si>
+    <t>DLink-XXXXXX</t>
   </si>
 </sst>
 </file>
@@ -390,8 +390,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -467,7 +471,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="73">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -502,6 +506,8 @@
     <cellStyle name="Hipervínculo" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -536,6 +542,8 @@
     <cellStyle name="Hipervínculo visitado" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -867,9 +875,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5:H7"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -900,13 +908,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -926,7 +934,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
@@ -949,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
@@ -960,19 +968,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
@@ -983,82 +991,82 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
@@ -1070,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1081,7 +1089,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>20</v>
@@ -1093,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1101,10 +1109,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>20</v>
@@ -1118,13 +1126,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
@@ -1136,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1153,7 +1161,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>11</v>
@@ -1164,16 +1172,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>20</v>
@@ -1182,18 +1190,18 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>20</v>
@@ -1205,21 +1213,21 @@
         <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>20</v>
@@ -1230,16 +1238,16 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>20</v>
@@ -1250,16 +1258,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>20</v>
@@ -1268,21 +1276,21 @@
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>20</v>
@@ -1293,16 +1301,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>20</v>
@@ -1316,10 +1324,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>20</v>
@@ -1353,36 +1361,36 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>20</v>
@@ -1394,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1419,16 +1427,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>20</v>
@@ -1439,13 +1447,13 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>20</v>
@@ -1459,16 +1467,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>20</v>
@@ -1479,16 +1487,16 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>20</v>
@@ -1499,13 +1507,13 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>20</v>
@@ -1519,16 +1527,16 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>20</v>
@@ -1539,39 +1547,39 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>20</v>
@@ -1582,16 +1590,16 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>20</v>
@@ -1602,16 +1610,16 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>20</v>
@@ -1622,16 +1630,16 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>20</v>
@@ -1642,16 +1650,16 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
@@ -1662,13 +1670,13 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>20</v>
@@ -1680,53 +1688,53 @@
         <v>0</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38" s="1">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1743,7 +1751,7 @@
         <v>11</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>11</v>
@@ -1752,18 +1760,18 @@
         <v>0</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>20</v>
@@ -1775,21 +1783,21 @@
         <v>0</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>20</v>
@@ -1798,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1815,7 +1823,7 @@
         <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>11</v>
@@ -1826,16 +1834,16 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>20</v>
@@ -1844,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1861,7 +1869,7 @@
         <v>11</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>11</v>
@@ -1884,7 +1892,7 @@
         <v>11</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>11</v>
@@ -1924,30 +1932,30 @@
         <v>19</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>20</v>
@@ -1959,18 +1967,18 @@
         <v>0</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>20</v>
@@ -1984,13 +1992,13 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Add all the bssids even unchecked ones for focusing on the interface for the next release.
</commit_message>
<xml_diff>
--- a/Supported networks.xlsx
+++ b/Supported networks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="25520" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="90">
   <si>
     <t>ESSID</t>
   </si>
@@ -147,15 +147,9 @@
     <t>Visto en routerkeygen</t>
   </si>
   <si>
-    <t>Yes?</t>
-  </si>
-  <si>
     <t>Any</t>
   </si>
   <si>
-    <t>HG265</t>
-  </si>
-  <si>
     <t>Visto en Telmex, HG530 (pero en vodafone no funciona!!!!!</t>
   </si>
   <si>
@@ -168,9 +162,6 @@
     <t>Por lo visto es el que tiene el Huawei U8100/8150, y otros routers</t>
   </si>
   <si>
-    <t>Visto en algunas Vodafone, pero tb en Orange</t>
-  </si>
-  <si>
     <t>Es de Orange, no comercializa ese router</t>
   </si>
   <si>
@@ -270,9 +261,6 @@
     <t>Es de Orange, no comercializa ese router… mac2wepkey http://pastebin.com/CgqMdXgC</t>
   </si>
   <si>
-    <t>WPA magic key</t>
-  </si>
-  <si>
     <t>Checked in internet</t>
   </si>
   <si>
@@ -301,6 +289,9 @@
   </si>
   <si>
     <t>DLink-XXXXXX</t>
+  </si>
+  <si>
+    <t>HG265, Visto en algunas Vodafone, pero tb en Orange</t>
   </si>
 </sst>
 </file>
@@ -387,8 +378,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,7 +529,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="143">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -514,6 +569,38 @@
     <cellStyle name="Hipervínculo" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -553,6 +640,38 @@
     <cellStyle name="Hipervínculo visitado" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -882,11 +1001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -920,10 +1039,10 @@
         <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
@@ -977,7 +1096,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
@@ -989,7 +1108,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>11</v>
@@ -1000,13 +1119,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
@@ -1018,18 +1137,18 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -1041,18 +1160,18 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1064,21 +1183,21 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
@@ -1087,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1109,9 +1228,6 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -1124,7 +1240,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>20</v>
@@ -1135,16 +1251,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>20</v>
@@ -1153,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1181,16 +1297,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>20</v>
@@ -1199,21 +1315,21 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>20</v>
@@ -1222,21 +1338,21 @@
         <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>20</v>
@@ -1247,16 +1363,16 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>20</v>
@@ -1267,39 +1383,39 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>20</v>
@@ -1310,16 +1426,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>20</v>
@@ -1339,7 +1455,7 @@
         <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
@@ -1359,7 +1475,7 @@
         <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>20</v>
@@ -1370,16 +1486,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>20</v>
@@ -1388,44 +1504,41 @@
         <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>20</v>
@@ -1436,16 +1549,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>20</v>
@@ -1456,16 +1569,16 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>20</v>
@@ -1476,16 +1589,16 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>20</v>
@@ -1496,36 +1609,39 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>20</v>
@@ -1536,16 +1652,16 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>20</v>
@@ -1556,39 +1672,36 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>20</v>
@@ -1599,16 +1712,16 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>20</v>
@@ -1619,99 +1732,111 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G35" s="1">
         <v>0</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="1">
         <v>0</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>81</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>20</v>
@@ -1720,21 +1845,21 @@
         <v>0</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>20</v>
@@ -1743,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1751,10 +1876,10 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>11</v>
@@ -1768,22 +1893,19 @@
       <c r="G40" s="1">
         <v>0</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>20</v>
@@ -1792,30 +1914,30 @@
         <v>0</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1823,10 +1945,10 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>11</v>
@@ -1843,16 +1965,16 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>20</v>
@@ -1861,161 +1983,92 @@
         <v>0</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F45" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G46" s="1">
         <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="1">
-        <v>0</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G50" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G51" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>